<commit_message>
[tsaipin] Add resilts of second try of CIT
</commit_message>
<xml_diff>
--- a/results/decentralized_permits.xlsx
+++ b/results/decentralized_permits.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annerosey/Documents/Projects/110-2PEA_Final/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA02131C-84F8-0442-A390-CAAEEFDF7EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6664EC98-F778-384B-AC85-5D9BB84E0580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="720" windowWidth="37320" windowHeight="17320" activeTab="1" xr2:uid="{5377F7A2-1FAD-A74D-94F0-59E8E0A58483}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="38000" windowHeight="19320" activeTab="1" xr2:uid="{5377F7A2-1FAD-A74D-94F0-59E8E0A58483}"/>
   </bookViews>
   <sheets>
     <sheet name="lambda" sheetId="1" r:id="rId1"/>
     <sheet name="x,y,b" sheetId="2" r:id="rId2"/>
     <sheet name="phi,a" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1768" uniqueCount="1765">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="1769">
   <si>
     <t>l[0,0]</t>
   </si>
@@ -5451,6 +5451,22 @@
   </si>
   <si>
     <t>16,20,23: 生產量增加且分配到的碳權增加，三種投入都增加。表示比較有環保效率，讓他多投入一點，產生一些</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>勞動成本</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他成本</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>垃圾處理量</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -5568,7 +5584,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5603,6 +5619,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -10554,27 +10573,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69981093-A304-544C-9DBE-1D56EB7B1A77}">
-  <dimension ref="A1:W73"/>
+  <dimension ref="A1:AG31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="4"/>
-    <col min="2" max="3" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="4"/>
-    <col min="7" max="9" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="10.83203125" style="4"/>
-    <col min="13" max="15" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="4"/>
+    <col min="2" max="3" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="14" width="13.5" style="4" customWidth="1"/>
+    <col min="15" max="16" width="10.83203125" style="4"/>
+    <col min="17" max="18" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="10.83203125" style="4"/>
+    <col min="23" max="25" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:27">
       <c r="B1" s="4" t="s">
-        <v>1756</v>
+        <v>1766</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1757</v>
@@ -10582,26 +10603,44 @@
       <c r="D1" s="4" t="s">
         <v>1758</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>1756</v>
+      <c r="G1" s="12" t="s">
+        <v>1767</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>1757</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>1758</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>1768</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>1757</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>1758</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>1756</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>1757</v>
+      </c>
+      <c r="S1" s="4" t="s">
         <v>1759</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>1760</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>1757</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>1761</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:27">
       <c r="A2" s="6" t="s">
         <v>576</v>
       </c>
@@ -10615,34 +10654,60 @@
         <f>B2-C2</f>
         <v>0</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>624</v>
+      <c r="F2" s="6" t="s">
+        <v>600</v>
       </c>
       <c r="G2" s="7">
-        <v>99631.87</v>
+        <v>1033323</v>
       </c>
       <c r="H2" s="5">
-        <v>99631.87</v>
+        <v>1033323</v>
       </c>
       <c r="I2" s="4">
         <f>G2-H2</f>
         <v>0</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="K2" s="7" t="s">
+        <v>1732</v>
+      </c>
+      <c r="L2" s="7">
+        <v>182263.4</v>
+      </c>
+      <c r="M2" s="5">
+        <v>182263.4</v>
+      </c>
+      <c r="N2" s="4">
+        <f>L2-M2</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>624</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>99631.87</v>
+      </c>
+      <c r="R2" s="5">
+        <v>99631.87</v>
+      </c>
+      <c r="S2" s="4">
+        <f>Q2-R2</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="9" t="s">
         <v>648</v>
       </c>
-      <c r="M2" s="7">
-        <v>0</v>
-      </c>
-      <c r="N2" s="5">
+      <c r="W2" s="7">
+        <v>0</v>
+      </c>
+      <c r="X2" s="5">
         <v>136697.54999999999</v>
       </c>
-      <c r="O2" s="4">
-        <f>N2-M2</f>
+      <c r="Y2" s="4">
+        <f>X2-W2</f>
         <v>136697.54999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:27">
       <c r="A3" s="6" t="s">
         <v>577</v>
       </c>
@@ -10656,34 +10721,60 @@
         <f t="shared" ref="D3:D66" si="0">B3-C3</f>
         <v>349621.29987353995</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="G3" s="7">
+        <v>2028040.2697992399</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1830292</v>
+      </c>
+      <c r="I3" s="4">
+        <f>G3-H3</f>
+        <v>197748.26979923993</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>1733</v>
+      </c>
+      <c r="L3" s="7">
+        <v>247742.54452853301</v>
+      </c>
+      <c r="M3" s="4">
+        <v>251500.79999999999</v>
+      </c>
+      <c r="N3" s="4">
+        <f>L3-M3</f>
+        <v>-3758.2554714669823</v>
+      </c>
+      <c r="P3" s="8" t="s">
         <v>625</v>
       </c>
-      <c r="G3" s="7">
+      <c r="Q3" s="7">
         <v>86535.904838365503</v>
       </c>
-      <c r="H3" s="4">
+      <c r="R3" s="4">
         <v>132776.5</v>
       </c>
-      <c r="I3" s="4">
-        <f t="shared" ref="I3:I25" si="1">G3-H3</f>
+      <c r="S3" s="4">
+        <f t="shared" ref="S3:S25" si="1">Q3-R3</f>
         <v>-46240.595161634497</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="V3" s="9" t="s">
         <v>649</v>
       </c>
-      <c r="M3" s="7">
+      <c r="W3" s="7">
         <v>2818.6916036009802</v>
       </c>
-      <c r="N3" s="4">
+      <c r="X3" s="4">
         <v>188625.59999999899</v>
       </c>
-      <c r="O3" s="4">
-        <f t="shared" ref="O3:O25" si="2">N3-M3</f>
+      <c r="Y3" s="4">
+        <f t="shared" ref="Y3:Y25" si="2">X3-W3</f>
         <v>185806.90839639801</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:27">
       <c r="A4" s="6" t="s">
         <v>578</v>
       </c>
@@ -10697,34 +10788,60 @@
         <f t="shared" si="0"/>
         <v>-107197.78144904505</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="G4" s="7">
+        <v>884349.64868630597</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1008138</v>
+      </c>
+      <c r="I4" s="4">
+        <f>G4-H4</f>
+        <v>-123788.35131369403</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>1734</v>
+      </c>
+      <c r="L4" s="7">
+        <v>149387.85605758999</v>
+      </c>
+      <c r="M4" s="4">
+        <v>146602.29999999999</v>
+      </c>
+      <c r="N4" s="4">
+        <f>L4-M4</f>
+        <v>2785.5560575900017</v>
+      </c>
+      <c r="P4" s="8" t="s">
         <v>626</v>
       </c>
-      <c r="G4" s="7">
+      <c r="Q4" s="7">
         <v>80070.358840896995</v>
       </c>
-      <c r="H4" s="4">
+      <c r="R4" s="4">
         <v>84818.29</v>
       </c>
-      <c r="I4" s="4">
+      <c r="S4" s="4">
         <f t="shared" si="1"/>
         <v>-4747.9311591029982</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="V4" s="9" t="s">
         <v>650</v>
       </c>
-      <c r="M4" s="7">
+      <c r="W4" s="7">
         <v>-2089.1670431941702</v>
       </c>
-      <c r="N4" s="4">
+      <c r="X4" s="4">
         <v>109951.724999999</v>
       </c>
-      <c r="O4" s="4">
+      <c r="Y4" s="4">
         <f t="shared" si="2"/>
         <v>112040.89204319318</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:27">
       <c r="A5" s="6" t="s">
         <v>579</v>
       </c>
@@ -10738,37 +10855,63 @@
         <f t="shared" si="0"/>
         <v>-1879082.42949317</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="G5" s="7">
+        <v>2408953.1866025501</v>
+      </c>
+      <c r="H5" s="4">
+        <v>5417133</v>
+      </c>
+      <c r="I5" s="4">
+        <f>G5-H5</f>
+        <v>-3008179.8133974499</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>1735</v>
+      </c>
+      <c r="L5" s="7">
+        <v>327887.29839934799</v>
+      </c>
+      <c r="M5" s="4">
+        <v>385843.3</v>
+      </c>
+      <c r="N5" s="4">
+        <f>L5-M5</f>
+        <v>-57956.001600652002</v>
+      </c>
+      <c r="P5" s="8" t="s">
         <v>627</v>
       </c>
-      <c r="G5" s="7">
+      <c r="Q5" s="7">
         <v>106051.42</v>
       </c>
-      <c r="H5" s="4">
+      <c r="R5" s="4">
         <v>235050.3</v>
       </c>
-      <c r="I5" s="4">
+      <c r="S5" s="4">
         <f t="shared" si="1"/>
         <v>-128998.87999999999</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="V5" s="9" t="s">
         <v>651</v>
       </c>
-      <c r="M5" s="7">
+      <c r="W5" s="7">
         <v>43467.0012004823</v>
       </c>
-      <c r="N5" s="4">
+      <c r="X5" s="4">
         <v>289382.47499999998</v>
       </c>
-      <c r="O5" s="4">
+      <c r="Y5" s="4">
         <f t="shared" si="2"/>
         <v>245915.47379951767</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="AA5" s="10" t="s">
         <v>1763</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:27">
       <c r="A6" s="6" t="s">
         <v>580</v>
       </c>
@@ -10782,37 +10925,63 @@
         <f t="shared" si="0"/>
         <v>1024001.22394143</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="G6" s="7">
+        <v>2282663.9509000899</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1083453</v>
+      </c>
+      <c r="I6" s="4">
+        <f>G6-H6</f>
+        <v>1199210.9509000899</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>1736</v>
+      </c>
+      <c r="L6" s="7">
+        <v>325151.13489429798</v>
+      </c>
+      <c r="M6" s="4">
+        <v>379717</v>
+      </c>
+      <c r="N6" s="4">
+        <f>L6-M6</f>
+        <v>-54565.865105702018</v>
+      </c>
+      <c r="P6" s="8" t="s">
         <v>628</v>
       </c>
-      <c r="G6" s="7">
+      <c r="Q6" s="7">
         <v>104913.28355135101</v>
       </c>
-      <c r="H6" s="4">
+      <c r="R6" s="4">
         <v>223770.7</v>
       </c>
-      <c r="I6" s="4">
+      <c r="S6" s="4">
         <f t="shared" si="1"/>
         <v>-118857.416448649</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="V6" s="9" t="s">
         <v>652</v>
       </c>
-      <c r="M6" s="7">
+      <c r="W6" s="7">
         <v>40924.398829281301</v>
       </c>
-      <c r="N6" s="4">
+      <c r="X6" s="4">
         <v>284787.75</v>
       </c>
-      <c r="O6" s="4">
+      <c r="Y6" s="4">
         <f t="shared" si="2"/>
         <v>243863.3511707187</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="AA6" s="11" t="s">
         <v>1764</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:27">
       <c r="A7" s="6" t="s">
         <v>581</v>
       </c>
@@ -10826,34 +10995,60 @@
         <f t="shared" si="0"/>
         <v>440729.48417776008</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1661516.4566589</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1083453</v>
+      </c>
+      <c r="I7" s="4">
+        <f>G7-H7</f>
+        <v>578063.45665890002</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>1737</v>
+      </c>
+      <c r="L7" s="7">
+        <v>304162.99278675101</v>
+      </c>
+      <c r="M7" s="4">
+        <v>327397.8</v>
+      </c>
+      <c r="N7" s="4">
+        <f>L7-M7</f>
+        <v>-23234.807213248976</v>
+      </c>
+      <c r="P7" s="8" t="s">
         <v>629</v>
       </c>
-      <c r="G7" s="7">
+      <c r="Q7" s="7">
         <v>106051.42</v>
       </c>
-      <c r="H7" s="4">
+      <c r="R7" s="4">
         <v>215609.2</v>
       </c>
-      <c r="I7" s="4">
+      <c r="S7" s="4">
         <f t="shared" si="1"/>
         <v>-109557.78000000001</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="V7" s="9" t="s">
         <v>653</v>
       </c>
-      <c r="M7" s="7">
+      <c r="W7" s="7">
         <v>17426.105409935099</v>
       </c>
-      <c r="N7" s="4">
+      <c r="X7" s="4">
         <v>245548.34999999899</v>
       </c>
-      <c r="O7" s="4">
+      <c r="Y7" s="4">
         <f t="shared" si="2"/>
         <v>228122.2445900639</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:27">
       <c r="A8" s="6" t="s">
         <v>582</v>
       </c>
@@ -10867,34 +11062,60 @@
         <f t="shared" si="0"/>
         <v>2.0395964384078979E-7</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="G8" s="7">
+        <v>1083453.0000002801</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1083453</v>
+      </c>
+      <c r="I8" s="4">
+        <f>G8-H8</f>
+        <v>2.8009526431560516E-7</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>1738</v>
+      </c>
+      <c r="L8" s="7">
+        <v>187722.29999999699</v>
+      </c>
+      <c r="M8" s="4">
+        <v>187722.3</v>
+      </c>
+      <c r="N8" s="4">
+        <f>L8-M8</f>
+        <v>-2.9976945370435715E-9</v>
+      </c>
+      <c r="P8" s="8" t="s">
         <v>630</v>
       </c>
-      <c r="G8" s="7">
+      <c r="Q8" s="7">
         <v>54236.189999947303</v>
       </c>
-      <c r="H8" s="4">
+      <c r="R8" s="4">
         <v>54236.19</v>
       </c>
-      <c r="I8" s="4">
+      <c r="S8" s="4">
         <f t="shared" si="1"/>
         <v>-5.2699760999530554E-8</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="V8" s="9" t="s">
         <v>654</v>
       </c>
-      <c r="M8" s="7">
-        <v>0</v>
-      </c>
-      <c r="N8" s="4">
+      <c r="W8" s="7">
+        <v>0</v>
+      </c>
+      <c r="X8" s="4">
         <v>140791.72499999899</v>
       </c>
-      <c r="O8" s="4">
+      <c r="Y8" s="4">
         <f t="shared" si="2"/>
         <v>140791.72499999899</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:27">
       <c r="A9" s="6" t="s">
         <v>583</v>
       </c>
@@ -10908,34 +11129,60 @@
         <f t="shared" si="0"/>
         <v>721453.66452991008</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="G9" s="7">
+        <v>2302880.3931623902</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1083453</v>
+      </c>
+      <c r="I9" s="4">
+        <f>G9-H9</f>
+        <v>1219427.3931623902</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>1739</v>
+      </c>
+      <c r="L9" s="7">
+        <v>370033.77948718</v>
+      </c>
+      <c r="M9" s="4">
+        <v>377061.7</v>
+      </c>
+      <c r="N9" s="4">
+        <f>L9-M9</f>
+        <v>-7027.9205128200119</v>
+      </c>
+      <c r="P9" s="8" t="s">
         <v>631</v>
       </c>
-      <c r="G9" s="7">
+      <c r="Q9" s="7">
         <v>106051.42</v>
       </c>
-      <c r="H9" s="4">
+      <c r="R9" s="4">
         <v>212407.2</v>
       </c>
-      <c r="I9" s="4">
+      <c r="S9" s="4">
         <f t="shared" si="1"/>
         <v>-106355.78000000001</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="V9" s="9" t="s">
         <v>655</v>
       </c>
-      <c r="M9" s="7">
+      <c r="W9" s="7">
         <v>5270.9403846114901</v>
       </c>
-      <c r="N9" s="4">
+      <c r="X9" s="4">
         <v>282796.27500000002</v>
       </c>
-      <c r="O9" s="4">
+      <c r="Y9" s="4">
         <f t="shared" si="2"/>
         <v>277525.33461538854</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:27">
       <c r="A10" s="6" t="s">
         <v>584</v>
       </c>
@@ -10949,34 +11196,60 @@
         <f t="shared" si="0"/>
         <v>839816.1496043501</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="G10" s="7">
+        <v>1309934.20487141</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1096798</v>
+      </c>
+      <c r="I10" s="4">
+        <f>G10-H10</f>
+        <v>213136.20487141004</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>1740</v>
+      </c>
+      <c r="L10" s="7">
+        <v>169646.061350148</v>
+      </c>
+      <c r="M10" s="4">
+        <v>177873.5</v>
+      </c>
+      <c r="N10" s="4">
+        <f>L10-M10</f>
+        <v>-8227.4386498520034</v>
+      </c>
+      <c r="P10" s="8" t="s">
         <v>632</v>
       </c>
-      <c r="G10" s="7">
+      <c r="Q10" s="7">
         <v>63046.503438427302</v>
       </c>
-      <c r="H10" s="4">
+      <c r="R10" s="4">
         <v>114549.6</v>
       </c>
-      <c r="I10" s="4">
+      <c r="S10" s="4">
         <f t="shared" si="1"/>
         <v>-51503.096561572704</v>
       </c>
-      <c r="L10" s="9" t="s">
+      <c r="V10" s="9" t="s">
         <v>656</v>
       </c>
-      <c r="M10" s="7">
+      <c r="W10" s="7">
         <v>6170.5789873898002</v>
       </c>
-      <c r="N10" s="4">
+      <c r="X10" s="4">
         <v>133405.125</v>
       </c>
-      <c r="O10" s="4">
+      <c r="Y10" s="4">
         <f t="shared" si="2"/>
         <v>127234.5460126102</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:27">
       <c r="A11" s="6" t="s">
         <v>585</v>
       </c>
@@ -10990,34 +11263,60 @@
         <f t="shared" si="0"/>
         <v>-730741.87417068006</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="G11" s="7">
+        <v>2360736.4741554302</v>
+      </c>
+      <c r="H11" s="4">
+        <v>3002925.66666666</v>
+      </c>
+      <c r="I11" s="4">
+        <f>G11-H11</f>
+        <v>-642189.19251122978</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>1741</v>
+      </c>
+      <c r="L11" s="7">
+        <v>327565.22512257198</v>
+      </c>
+      <c r="M11" s="4">
+        <v>379168.7</v>
+      </c>
+      <c r="N11" s="4">
+        <f>L11-M11</f>
+        <v>-51603.474877428031</v>
+      </c>
+      <c r="P11" s="8" t="s">
         <v>633</v>
       </c>
-      <c r="G11" s="7">
+      <c r="Q11" s="7">
         <v>106051.42</v>
       </c>
-      <c r="H11" s="4">
+      <c r="R11" s="4">
         <v>134504.29999999999</v>
       </c>
-      <c r="I11" s="4">
+      <c r="S11" s="4">
         <f t="shared" si="1"/>
         <v>-28452.87999999999</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="V11" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="M11" s="7">
+      <c r="W11" s="7">
         <v>38702.606158077702</v>
       </c>
-      <c r="N11" s="4">
+      <c r="X11" s="4">
         <v>284376.52500000002</v>
       </c>
-      <c r="O11" s="4">
+      <c r="Y11" s="4">
         <f t="shared" si="2"/>
         <v>245673.91884192231</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:27">
       <c r="A12" s="6" t="s">
         <v>586</v>
       </c>
@@ -11031,34 +11330,60 @@
         <f t="shared" si="0"/>
         <v>-1329617.3392680699</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="G12" s="7">
+        <v>1945923.0416785199</v>
+      </c>
+      <c r="H12" s="4">
+        <v>3002925.66666666</v>
+      </c>
+      <c r="I12" s="4">
+        <f>G12-H12</f>
+        <v>-1057002.6249881401</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>1742</v>
+      </c>
+      <c r="L12" s="7">
+        <v>231412.59129228999</v>
+      </c>
+      <c r="M12" s="4">
+        <v>202365.1</v>
+      </c>
+      <c r="N12" s="4">
+        <f>L12-M12</f>
+        <v>29047.491292289982</v>
+      </c>
+      <c r="P12" s="8" t="s">
         <v>634</v>
       </c>
-      <c r="G12" s="7">
+      <c r="Q12" s="7">
         <v>99051.871479902606</v>
       </c>
-      <c r="H12" s="4">
+      <c r="R12" s="4">
         <v>102684.9</v>
       </c>
-      <c r="I12" s="4">
+      <c r="S12" s="4">
         <f t="shared" si="1"/>
         <v>-3633.0285200973885</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="V12" s="9" t="s">
         <v>658</v>
       </c>
-      <c r="M12" s="7">
+      <c r="W12" s="7">
         <v>-21785.618469223398</v>
       </c>
-      <c r="N12" s="4">
+      <c r="X12" s="4">
         <v>151773.82500000001</v>
       </c>
-      <c r="O12" s="4">
+      <c r="Y12" s="4">
         <f t="shared" si="2"/>
         <v>173559.44346922342</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:27">
       <c r="A13" s="6" t="s">
         <v>587</v>
       </c>
@@ -11072,34 +11397,60 @@
         <f t="shared" si="0"/>
         <v>-558172.39567568991</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="G13" s="7">
+        <v>3241875.2846392901</v>
+      </c>
+      <c r="H13" s="4">
+        <v>3002925.66666666</v>
+      </c>
+      <c r="I13" s="4">
+        <f>G13-H13</f>
+        <v>238949.61797263008</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>1743</v>
+      </c>
+      <c r="L13" s="7">
+        <v>330041.53155761398</v>
+      </c>
+      <c r="M13" s="4">
+        <v>251888.9</v>
+      </c>
+      <c r="N13" s="4">
+        <f>L13-M13</f>
+        <v>78152.63155761399</v>
+      </c>
+      <c r="P13" s="8" t="s">
         <v>635</v>
       </c>
-      <c r="G13" s="7">
+      <c r="Q13" s="7">
         <v>106051.42</v>
       </c>
-      <c r="H13" s="4">
+      <c r="R13" s="4">
         <v>123818.5</v>
       </c>
-      <c r="I13" s="4">
+      <c r="S13" s="4">
         <f t="shared" si="1"/>
         <v>-17767.080000000002</v>
       </c>
-      <c r="L13" s="9" t="s">
+      <c r="V13" s="9" t="s">
         <v>659</v>
       </c>
-      <c r="M13" s="7">
+      <c r="W13" s="7">
         <v>-58614.473668217703</v>
       </c>
-      <c r="N13" s="4">
+      <c r="X13" s="4">
         <v>188916.67499999999</v>
       </c>
-      <c r="O13" s="4">
+      <c r="Y13" s="4">
         <f t="shared" si="2"/>
         <v>247531.14866821771</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:27">
       <c r="A14" s="6" t="s">
         <v>588</v>
       </c>
@@ -11113,34 +11464,60 @@
         <f t="shared" si="0"/>
         <v>321994.55147932202</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="G14" s="7">
+        <v>1203114.89828312</v>
+      </c>
+      <c r="H14" s="4">
+        <v>976738</v>
+      </c>
+      <c r="I14" s="4">
+        <f>G14-H14</f>
+        <v>226376.89828312001</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="L14" s="7">
+        <v>187914.124263039</v>
+      </c>
+      <c r="M14" s="4">
+        <v>219906.8</v>
+      </c>
+      <c r="N14" s="4">
+        <f>L14-M14</f>
+        <v>-31992.675736960984</v>
+      </c>
+      <c r="P14" s="8" t="s">
         <v>636</v>
       </c>
-      <c r="G14" s="7">
+      <c r="Q14" s="7">
         <v>53870.8719565922</v>
       </c>
-      <c r="H14" s="4">
+      <c r="R14" s="4">
         <v>134164.5</v>
       </c>
-      <c r="I14" s="4">
+      <c r="S14" s="4">
         <f t="shared" si="1"/>
         <v>-80293.628043407807</v>
       </c>
-      <c r="L14" s="9" t="s">
+      <c r="V14" s="9" t="s">
         <v>660</v>
       </c>
-      <c r="M14" s="7">
+      <c r="W14" s="7">
         <v>23994.506802722801</v>
       </c>
-      <c r="N14" s="4">
+      <c r="X14" s="4">
         <v>164930.09999999899</v>
       </c>
-      <c r="O14" s="4">
+      <c r="Y14" s="4">
         <f t="shared" si="2"/>
         <v>140935.59319727618</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:27">
       <c r="A15" s="6" t="s">
         <v>589</v>
       </c>
@@ -11154,34 +11531,60 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="6" t="s">
+        <v>613</v>
+      </c>
+      <c r="G15" s="7">
+        <v>776203</v>
+      </c>
+      <c r="H15" s="4">
+        <v>776203</v>
+      </c>
+      <c r="I15" s="4">
+        <f>G15-H15</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>1745</v>
+      </c>
+      <c r="L15" s="7">
+        <v>63239.45</v>
+      </c>
+      <c r="M15" s="4">
+        <v>63239.45</v>
+      </c>
+      <c r="N15" s="4">
+        <f>L15-M15</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="8" t="s">
         <v>637</v>
       </c>
-      <c r="G15" s="7">
+      <c r="Q15" s="7">
         <v>16811.61</v>
       </c>
-      <c r="H15" s="4">
+      <c r="R15" s="4">
         <v>16811.61</v>
       </c>
-      <c r="I15" s="4">
+      <c r="S15" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="V15" s="9" t="s">
         <v>661</v>
       </c>
-      <c r="M15" s="7">
-        <v>0</v>
-      </c>
-      <c r="N15" s="4">
+      <c r="W15" s="7">
+        <v>0</v>
+      </c>
+      <c r="X15" s="4">
         <v>47429.5874999999</v>
       </c>
-      <c r="O15" s="4">
+      <c r="Y15" s="4">
         <f t="shared" si="2"/>
         <v>47429.5874999999</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:27">
       <c r="A16" s="6" t="s">
         <v>590</v>
       </c>
@@ -11195,34 +11598,60 @@
         <f t="shared" si="0"/>
         <v>417310.97179641994</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="G16" s="7">
+        <v>1361336.4543498701</v>
+      </c>
+      <c r="H16" s="4">
+        <v>871609</v>
+      </c>
+      <c r="I16" s="4">
+        <f>G16-H16</f>
+        <v>489727.4543498701</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>1746</v>
+      </c>
+      <c r="L16" s="7">
+        <v>207404.68200887501</v>
+      </c>
+      <c r="M16" s="4">
+        <v>268204.2</v>
+      </c>
+      <c r="N16" s="4">
+        <f>L16-M16</f>
+        <v>-60799.517991125002</v>
+      </c>
+      <c r="P16" s="8" t="s">
         <v>638</v>
       </c>
-      <c r="G16" s="7">
+      <c r="Q16" s="7">
         <v>64956.241432029099</v>
       </c>
-      <c r="H16" s="4">
+      <c r="R16" s="4">
         <v>157251.29999999999</v>
       </c>
-      <c r="I16" s="4">
+      <c r="S16" s="4">
         <f t="shared" si="1"/>
         <v>-92295.058567970889</v>
       </c>
-      <c r="L16" s="9" t="s">
+      <c r="V16" s="9" t="s">
         <v>662</v>
       </c>
-      <c r="M16" s="7">
+      <c r="W16" s="7">
         <v>45599.638493344202</v>
       </c>
-      <c r="N16" s="4">
+      <c r="X16" s="4">
         <v>201153.15</v>
       </c>
-      <c r="O16" s="4">
+      <c r="Y16" s="4">
         <f t="shared" si="2"/>
         <v>155553.51150665578</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:33">
       <c r="A17" s="6" t="s">
         <v>591</v>
       </c>
@@ -11236,34 +11665,60 @@
         <f t="shared" si="0"/>
         <v>281005.30219200999</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="6" t="s">
+        <v>615</v>
+      </c>
+      <c r="G17" s="7">
+        <v>2026103.86514649</v>
+      </c>
+      <c r="H17" s="4">
+        <v>1623739</v>
+      </c>
+      <c r="I17" s="4">
+        <f>G17-H17</f>
+        <v>402364.86514649005</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>1747</v>
+      </c>
+      <c r="L17" s="7">
+        <v>248116.36358876101</v>
+      </c>
+      <c r="M17" s="4">
+        <v>254156.7</v>
+      </c>
+      <c r="N17" s="4">
+        <f>L17-M17</f>
+        <v>-6040.3364112389972</v>
+      </c>
+      <c r="P17" s="8" t="s">
         <v>639</v>
       </c>
-      <c r="G17" s="7">
+      <c r="Q17" s="7">
         <v>86768.484884998397</v>
       </c>
-      <c r="H17" s="4">
+      <c r="R17" s="4">
         <v>131201.5</v>
       </c>
-      <c r="I17" s="4">
+      <c r="S17" s="4">
         <f t="shared" si="1"/>
         <v>-44433.015115001603</v>
       </c>
-      <c r="L17" s="9" t="s">
+      <c r="V17" s="9" t="s">
         <v>663</v>
       </c>
-      <c r="M17" s="7">
+      <c r="W17" s="7">
         <v>4530.2523084282902</v>
       </c>
-      <c r="N17" s="4">
+      <c r="X17" s="4">
         <v>190617.52499999999</v>
       </c>
-      <c r="O17" s="4">
+      <c r="Y17" s="4">
         <f t="shared" si="2"/>
         <v>186087.27269157171</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:33">
       <c r="A18" s="6" t="s">
         <v>592</v>
       </c>
@@ -11277,34 +11732,60 @@
         <f t="shared" si="0"/>
         <v>-311510.93803078006</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="G18" s="7">
+        <v>2017510.49024682</v>
+      </c>
+      <c r="H18" s="4">
+        <v>1898015.33333333</v>
+      </c>
+      <c r="I18" s="4">
+        <f>G18-H18</f>
+        <v>119495.15691349003</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="L18" s="7">
+        <v>223151.29775079599</v>
+      </c>
+      <c r="M18" s="4">
+        <v>182567.5</v>
+      </c>
+      <c r="N18" s="4">
+        <f>L18-M18</f>
+        <v>40583.797750795988</v>
+      </c>
+      <c r="P18" s="8" t="s">
         <v>640</v>
       </c>
-      <c r="G18" s="7">
+      <c r="Q18" s="7">
         <v>89995.348541003201</v>
       </c>
-      <c r="H18" s="4">
+      <c r="R18" s="4">
         <v>72399.38</v>
       </c>
-      <c r="I18" s="4">
+      <c r="S18" s="4">
         <f t="shared" si="1"/>
         <v>17595.968541003196</v>
       </c>
-      <c r="L18" s="9" t="s">
+      <c r="V18" s="9" t="s">
         <v>664</v>
       </c>
-      <c r="M18" s="7">
+      <c r="W18" s="7">
         <v>-30437.8483130932</v>
       </c>
-      <c r="N18" s="4">
+      <c r="X18" s="4">
         <v>136925.625</v>
       </c>
-      <c r="O18" s="4">
+      <c r="Y18" s="4">
         <f t="shared" si="2"/>
         <v>167363.47331309319</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:33">
       <c r="A19" s="6" t="s">
         <v>593</v>
       </c>
@@ -11318,37 +11799,63 @@
         <f t="shared" si="0"/>
         <v>99405.398981180042</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="G19" s="7">
+        <v>1879347.06328208</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1898015.33333333</v>
+      </c>
+      <c r="I19" s="4">
+        <f>G19-H19</f>
+        <v>-18668.270051250001</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>1749</v>
+      </c>
+      <c r="L19" s="7">
+        <v>256357.55055047799</v>
+      </c>
+      <c r="M19" s="4">
+        <v>262122.4</v>
+      </c>
+      <c r="N19" s="4">
+        <f t="shared" ref="N19:N25" si="3">L19-M19</f>
+        <v>-5764.8494495220075</v>
+      </c>
+      <c r="P19" s="8" t="s">
         <v>641</v>
       </c>
-      <c r="G19" s="7">
+      <c r="Q19" s="7">
         <v>106051.42</v>
       </c>
-      <c r="H19" s="4">
+      <c r="R19" s="4">
         <v>160709</v>
       </c>
-      <c r="I19" s="4">
+      <c r="S19" s="4">
         <f t="shared" si="1"/>
         <v>-54657.58</v>
       </c>
-      <c r="L19" s="9" t="s">
+      <c r="V19" s="9" t="s">
         <v>665</v>
       </c>
-      <c r="M19" s="7">
+      <c r="W19" s="7">
         <v>4323.6370871365098</v>
       </c>
-      <c r="N19" s="4">
+      <c r="X19" s="4">
         <v>196591.8</v>
       </c>
-      <c r="O19" s="4">
+      <c r="Y19" s="4">
         <f t="shared" si="2"/>
         <v>192268.16291286348</v>
       </c>
-      <c r="W19" s="4" t="s">
+      <c r="AG19" s="4" t="s">
         <v>1762</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:33">
       <c r="A20" s="6" t="s">
         <v>594</v>
       </c>
@@ -11362,34 +11869,60 @@
         <f t="shared" si="0"/>
         <v>-691362.34496814304</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="G20" s="7">
+        <v>1278407.7781017199</v>
+      </c>
+      <c r="H20" s="4">
+        <v>1898015.33333333</v>
+      </c>
+      <c r="I20" s="4">
+        <f>G20-H20</f>
+        <v>-619607.55523161008</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>1750</v>
+      </c>
+      <c r="L20" s="7">
+        <v>188034.822675737</v>
+      </c>
+      <c r="M20" s="4">
+        <v>271807.09999999998</v>
+      </c>
+      <c r="N20" s="4">
+        <f t="shared" si="3"/>
+        <v>-83772.277324262977</v>
+      </c>
+      <c r="P20" s="8" t="s">
         <v>642</v>
       </c>
-      <c r="G20" s="7">
+      <c r="Q20" s="7">
         <v>53641.008918043401</v>
       </c>
-      <c r="H20" s="4">
+      <c r="R20" s="4">
         <v>168598.7</v>
       </c>
-      <c r="I20" s="4">
+      <c r="S20" s="4">
         <f t="shared" si="1"/>
         <v>-114957.69108195661</v>
       </c>
-      <c r="L20" s="9" t="s">
+      <c r="V20" s="9" t="s">
         <v>666</v>
       </c>
-      <c r="M20" s="7">
+      <c r="W20" s="7">
         <v>62829.207993194497</v>
       </c>
-      <c r="N20" s="4">
+      <c r="X20" s="4">
         <v>203855.32499999899</v>
       </c>
-      <c r="O20" s="4">
+      <c r="Y20" s="4">
         <f t="shared" si="2"/>
         <v>141026.1170068045</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:33">
       <c r="A21" s="6" t="s">
         <v>595</v>
       </c>
@@ -11403,34 +11936,60 @@
         <f t="shared" si="0"/>
         <v>9.8953023552894592E-10</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="G21" s="7">
+        <v>2409203.3333333302</v>
+      </c>
+      <c r="H21" s="4">
+        <v>2409203.3333333302</v>
+      </c>
+      <c r="I21" s="4">
+        <f>G21-H21</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>1751</v>
+      </c>
+      <c r="L21" s="7">
+        <v>134966.79999999999</v>
+      </c>
+      <c r="M21" s="4">
+        <v>134966.79999999999</v>
+      </c>
+      <c r="N21" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P21" s="8" t="s">
         <v>643</v>
       </c>
-      <c r="G21" s="7">
+      <c r="Q21" s="7">
         <v>30631.83</v>
       </c>
-      <c r="H21" s="4">
+      <c r="R21" s="4">
         <v>30631.83</v>
       </c>
-      <c r="I21" s="4">
+      <c r="S21" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L21" s="9" t="s">
+      <c r="V21" s="9" t="s">
         <v>667</v>
       </c>
-      <c r="M21" s="7">
-        <v>0</v>
-      </c>
-      <c r="N21" s="4">
+      <c r="W21" s="7">
+        <v>0</v>
+      </c>
+      <c r="X21" s="4">
         <v>101225.099999999</v>
       </c>
-      <c r="O21" s="4">
+      <c r="Y21" s="4">
         <f t="shared" si="2"/>
         <v>101225.099999999</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:33">
       <c r="A22" s="6" t="s">
         <v>596</v>
       </c>
@@ -11444,34 +12003,60 @@
         <f t="shared" si="0"/>
         <v>1501438.2766887939</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="G22" s="7">
+        <v>3844804.23299347</v>
+      </c>
+      <c r="H22" s="4">
+        <v>2409203.3333333302</v>
+      </c>
+      <c r="I22" s="4">
+        <f>G22-H22</f>
+        <v>1435600.8996601398</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>1752</v>
+      </c>
+      <c r="L22" s="7">
+        <v>323187.666426257</v>
+      </c>
+      <c r="M22" s="4">
+        <v>216178.4</v>
+      </c>
+      <c r="N22" s="4">
+        <f t="shared" si="3"/>
+        <v>107009.266426257</v>
+      </c>
+      <c r="P22" s="8" t="s">
         <v>644</v>
       </c>
-      <c r="G22" s="7">
+      <c r="Q22" s="7">
         <v>88407.296872035993</v>
       </c>
-      <c r="H22" s="4">
+      <c r="R22" s="4">
         <v>79307.77</v>
       </c>
-      <c r="I22" s="4">
+      <c r="S22" s="4">
         <f t="shared" si="1"/>
         <v>9099.5268720359891</v>
       </c>
-      <c r="L22" s="9" t="s">
+      <c r="V22" s="9" t="s">
         <v>668</v>
       </c>
-      <c r="M22" s="7">
+      <c r="W22" s="7">
         <v>-80256.949819698901</v>
       </c>
-      <c r="N22" s="4">
+      <c r="X22" s="4">
         <v>162133.79999999999</v>
       </c>
-      <c r="O22" s="4">
+      <c r="Y22" s="4">
         <f t="shared" si="2"/>
         <v>242390.74981969889</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:33">
       <c r="A23" s="6" t="s">
         <v>597</v>
       </c>
@@ -11485,34 +12070,60 @@
         <f t="shared" si="0"/>
         <v>1296039.232138054</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="6" t="s">
+        <v>621</v>
+      </c>
+      <c r="G23" s="7">
+        <v>2571161.7245281599</v>
+      </c>
+      <c r="H23" s="4">
+        <v>2409203.3333333302</v>
+      </c>
+      <c r="I23" s="4">
+        <f>G23-H23</f>
+        <v>161958.39119482972</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>1753</v>
+      </c>
+      <c r="L23" s="7">
+        <v>372762.24272085499</v>
+      </c>
+      <c r="M23" s="4">
+        <v>356538</v>
+      </c>
+      <c r="N23" s="4">
+        <f t="shared" si="3"/>
+        <v>16224.242720854993</v>
+      </c>
+      <c r="P23" s="8" t="s">
         <v>645</v>
       </c>
-      <c r="G23" s="7">
+      <c r="Q23" s="7">
         <v>106051.42</v>
       </c>
-      <c r="H23" s="4">
+      <c r="R23" s="4">
         <v>179905</v>
       </c>
-      <c r="I23" s="4">
+      <c r="S23" s="4">
         <f t="shared" si="1"/>
         <v>-73853.58</v>
       </c>
-      <c r="L23" s="9" t="s">
+      <c r="V23" s="9" t="s">
         <v>669</v>
       </c>
-      <c r="M23" s="7">
+      <c r="W23" s="7">
         <v>-12168.1820406467</v>
       </c>
-      <c r="N23" s="4">
+      <c r="X23" s="4">
         <v>267403.5</v>
       </c>
-      <c r="O23" s="4">
+      <c r="Y23" s="4">
         <f t="shared" si="2"/>
         <v>279571.68204064667</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:33">
       <c r="A24" s="6" t="s">
         <v>598</v>
       </c>
@@ -11526,34 +12137,60 @@
         <f t="shared" si="0"/>
         <v>567435.79987353995</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="G24" s="7">
+        <v>2028040.2697992399</v>
+      </c>
+      <c r="H24" s="4">
+        <v>1429848.5</v>
+      </c>
+      <c r="I24" s="4">
+        <f>G24-H24</f>
+        <v>598191.76979923993</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>1754</v>
+      </c>
+      <c r="L24" s="7">
+        <v>247742.54452853301</v>
+      </c>
+      <c r="M24" s="4">
+        <v>251192.7</v>
+      </c>
+      <c r="N24" s="4">
+        <f t="shared" si="3"/>
+        <v>-3450.1554714670056</v>
+      </c>
+      <c r="P24" s="8" t="s">
         <v>646</v>
       </c>
-      <c r="G24" s="7">
+      <c r="Q24" s="7">
         <v>86535.904838365503</v>
       </c>
-      <c r="H24" s="4">
+      <c r="R24" s="4">
         <v>149915.29999999999</v>
       </c>
-      <c r="I24" s="4">
+      <c r="S24" s="4">
         <f t="shared" si="1"/>
         <v>-63379.395161634486</v>
       </c>
-      <c r="L24" s="9" t="s">
+      <c r="V24" s="9" t="s">
         <v>670</v>
       </c>
-      <c r="M24" s="7">
+      <c r="W24" s="7">
         <v>2587.616603598</v>
       </c>
-      <c r="N24" s="4">
+      <c r="X24" s="4">
         <v>188394.52499999999</v>
       </c>
-      <c r="O24" s="4">
+      <c r="Y24" s="4">
         <f t="shared" si="2"/>
         <v>185806.908396402</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:33">
       <c r="A25" s="6" t="s">
         <v>599</v>
       </c>
@@ -11567,770 +12204,89 @@
         <f t="shared" si="0"/>
         <v>136394.26393312006</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="G25" s="7">
+        <v>1950352.0607086001</v>
+      </c>
+      <c r="H25" s="4">
+        <v>1429848.5</v>
+      </c>
+      <c r="I25" s="4">
+        <f>G25-H25</f>
+        <v>520503.5607086001</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>1755</v>
+      </c>
+      <c r="L25" s="7">
+        <v>230368.63951035001</v>
+      </c>
+      <c r="M25" s="4">
+        <v>164930.20000000001</v>
+      </c>
+      <c r="N25" s="4">
+        <f t="shared" si="3"/>
+        <v>65438.439510349999</v>
+      </c>
+      <c r="P25" s="8" t="s">
         <v>647</v>
       </c>
-      <c r="G25" s="7">
+      <c r="Q25" s="7">
         <v>98535.480408041403</v>
       </c>
-      <c r="H25" s="4">
+      <c r="R25" s="4">
         <v>73605.600000000006</v>
       </c>
-      <c r="I25" s="4">
+      <c r="S25" s="4">
         <f t="shared" si="1"/>
         <v>24929.880408041397</v>
       </c>
-      <c r="L25" s="9" t="s">
+      <c r="V25" s="9" t="s">
         <v>671</v>
       </c>
-      <c r="M25" s="7">
+      <c r="W25" s="7">
         <v>-49078.829632759102</v>
       </c>
-      <c r="N25" s="4">
+      <c r="X25" s="4">
         <v>123697.65</v>
       </c>
-      <c r="O25" s="4">
+      <c r="Y25" s="4">
         <f t="shared" si="2"/>
         <v>172776.47963275909</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
-      <c r="A26" s="6" t="s">
-        <v>600</v>
-      </c>
-      <c r="B26" s="7">
-        <v>1033323</v>
-      </c>
-      <c r="C26" s="5">
-        <v>1033323</v>
-      </c>
-      <c r="D26" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="4">
-        <f>SUM(G2:G25)</f>
+    <row r="26" spans="1:33">
+      <c r="Q26" s="4">
+        <f>SUM(Q2:Q25)</f>
         <v>2000000.0000000002</v>
       </c>
-      <c r="N26" s="4">
-        <f>SUM(N2:N25)</f>
+      <c r="V26" s="4" t="s">
+        <v>1765</v>
+      </c>
+      <c r="W26" s="4">
+        <f>SUM(W2:W25)</f>
+        <v>44214.112874969804</v>
+      </c>
+      <c r="X26" s="4">
+        <f>SUM(X2:X25)</f>
         <v>4421411.2874999931</v>
       </c>
-      <c r="O26" s="4">
-        <f>SUM(O2:O25)</f>
+      <c r="Y26" s="4">
+        <f>SUM(Y2:Y25)</f>
         <v>4377197.1746250233</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
-      <c r="A27" s="6" t="s">
-        <v>601</v>
-      </c>
-      <c r="B27" s="7">
-        <v>2028040.2697992399</v>
-      </c>
-      <c r="C27" s="4">
-        <v>1830292</v>
-      </c>
-      <c r="D27" s="4">
-        <f t="shared" si="0"/>
-        <v>197748.26979923993</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23">
-      <c r="A28" s="6" t="s">
-        <v>602</v>
-      </c>
-      <c r="B28" s="7">
-        <v>884349.64868630597</v>
-      </c>
-      <c r="C28" s="4">
-        <v>1008138</v>
-      </c>
-      <c r="D28" s="4">
-        <f t="shared" si="0"/>
-        <v>-123788.35131369403</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23">
-      <c r="A29" s="6" t="s">
-        <v>603</v>
-      </c>
-      <c r="B29" s="7">
-        <v>2408953.1866025501</v>
-      </c>
-      <c r="C29" s="4">
-        <v>5417133</v>
-      </c>
-      <c r="D29" s="4">
-        <f t="shared" si="0"/>
-        <v>-3008179.8133974499</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23">
-      <c r="A30" s="6" t="s">
-        <v>604</v>
-      </c>
-      <c r="B30" s="7">
-        <v>2282663.9509000899</v>
-      </c>
-      <c r="C30" s="4">
-        <v>1083453</v>
-      </c>
-      <c r="D30" s="4">
-        <f t="shared" si="0"/>
-        <v>1199210.9509000899</v>
-      </c>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:23">
-      <c r="A31" s="6" t="s">
-        <v>605</v>
-      </c>
-      <c r="B31" s="7">
-        <v>1661516.4566589</v>
-      </c>
-      <c r="C31" s="4">
-        <v>1083453</v>
-      </c>
-      <c r="D31" s="4">
-        <f t="shared" si="0"/>
-        <v>578063.45665890002</v>
-      </c>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:23">
-      <c r="A32" s="6" t="s">
-        <v>606</v>
-      </c>
-      <c r="B32" s="7">
-        <v>1083453.0000002801</v>
-      </c>
-      <c r="C32" s="4">
-        <v>1083453</v>
-      </c>
-      <c r="D32" s="4">
-        <f t="shared" si="0"/>
-        <v>2.8009526431560516E-7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="6" t="s">
-        <v>607</v>
-      </c>
-      <c r="B33" s="7">
-        <v>2302880.3931623902</v>
-      </c>
-      <c r="C33" s="4">
-        <v>1083453</v>
-      </c>
-      <c r="D33" s="4">
-        <f t="shared" si="0"/>
-        <v>1219427.3931623902</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="6" t="s">
-        <v>608</v>
-      </c>
-      <c r="B34" s="7">
-        <v>1309934.20487141</v>
-      </c>
-      <c r="C34" s="4">
-        <v>1096798</v>
-      </c>
-      <c r="D34" s="4">
-        <f t="shared" si="0"/>
-        <v>213136.20487141004</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="6" t="s">
-        <v>609</v>
-      </c>
-      <c r="B35" s="7">
-        <v>2360736.4741554302</v>
-      </c>
-      <c r="C35" s="4">
-        <v>3002925.66666666</v>
-      </c>
-      <c r="D35" s="4">
-        <f t="shared" si="0"/>
-        <v>-642189.19251122978</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="6" t="s">
-        <v>610</v>
-      </c>
-      <c r="B36" s="7">
-        <v>1945923.0416785199</v>
-      </c>
-      <c r="C36" s="4">
-        <v>3002925.66666666</v>
-      </c>
-      <c r="D36" s="4">
-        <f t="shared" si="0"/>
-        <v>-1057002.6249881401</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="6" t="s">
-        <v>611</v>
-      </c>
-      <c r="B37" s="7">
-        <v>3241875.2846392901</v>
-      </c>
-      <c r="C37" s="4">
-        <v>3002925.66666666</v>
-      </c>
-      <c r="D37" s="4">
-        <f t="shared" si="0"/>
-        <v>238949.61797263008</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="6" t="s">
-        <v>612</v>
-      </c>
-      <c r="B38" s="7">
-        <v>1203114.89828312</v>
-      </c>
-      <c r="C38" s="4">
-        <v>976738</v>
-      </c>
-      <c r="D38" s="4">
-        <f t="shared" si="0"/>
-        <v>226376.89828312001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="6" t="s">
-        <v>613</v>
-      </c>
-      <c r="B39" s="7">
-        <v>776203</v>
-      </c>
-      <c r="C39" s="4">
-        <v>776203</v>
-      </c>
-      <c r="D39" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="6" t="s">
-        <v>614</v>
-      </c>
-      <c r="B40" s="7">
-        <v>1361336.4543498701</v>
-      </c>
-      <c r="C40" s="4">
-        <v>871609</v>
-      </c>
-      <c r="D40" s="4">
-        <f t="shared" si="0"/>
-        <v>489727.4543498701</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="6" t="s">
-        <v>615</v>
-      </c>
-      <c r="B41" s="7">
-        <v>2026103.86514649</v>
-      </c>
-      <c r="C41" s="4">
-        <v>1623739</v>
-      </c>
-      <c r="D41" s="4">
-        <f t="shared" si="0"/>
-        <v>402364.86514649005</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="6" t="s">
-        <v>616</v>
-      </c>
-      <c r="B42" s="7">
-        <v>2017510.49024682</v>
-      </c>
-      <c r="C42" s="4">
-        <v>1898015.33333333</v>
-      </c>
-      <c r="D42" s="4">
-        <f t="shared" si="0"/>
-        <v>119495.15691349003</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="6" t="s">
-        <v>617</v>
-      </c>
-      <c r="B43" s="7">
-        <v>1879347.06328208</v>
-      </c>
-      <c r="C43" s="4">
-        <v>1898015.33333333</v>
-      </c>
-      <c r="D43" s="4">
-        <f t="shared" si="0"/>
-        <v>-18668.270051250001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="6" t="s">
-        <v>618</v>
-      </c>
-      <c r="B44" s="7">
-        <v>1278407.7781017199</v>
-      </c>
-      <c r="C44" s="4">
-        <v>1898015.33333333</v>
-      </c>
-      <c r="D44" s="4">
-        <f t="shared" si="0"/>
-        <v>-619607.55523161008</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="6" t="s">
-        <v>619</v>
-      </c>
-      <c r="B45" s="7">
-        <v>2409203.3333333302</v>
-      </c>
-      <c r="C45" s="4">
-        <v>2409203.3333333302</v>
-      </c>
-      <c r="D45" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="6" t="s">
-        <v>620</v>
-      </c>
-      <c r="B46" s="7">
-        <v>3844804.23299347</v>
-      </c>
-      <c r="C46" s="4">
-        <v>2409203.3333333302</v>
-      </c>
-      <c r="D46" s="4">
-        <f t="shared" si="0"/>
-        <v>1435600.8996601398</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="6" t="s">
-        <v>621</v>
-      </c>
-      <c r="B47" s="7">
-        <v>2571161.7245281599</v>
-      </c>
-      <c r="C47" s="4">
-        <v>2409203.3333333302</v>
-      </c>
-      <c r="D47" s="4">
-        <f t="shared" si="0"/>
-        <v>161958.39119482972</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="6" t="s">
-        <v>622</v>
-      </c>
-      <c r="B48" s="7">
-        <v>2028040.2697992399</v>
-      </c>
-      <c r="C48" s="4">
-        <v>1429848.5</v>
-      </c>
-      <c r="D48" s="4">
-        <f t="shared" si="0"/>
-        <v>598191.76979923993</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="6" t="s">
-        <v>623</v>
-      </c>
-      <c r="B49" s="7">
-        <v>1950352.0607086001</v>
-      </c>
-      <c r="C49" s="4">
-        <v>1429848.5</v>
-      </c>
-      <c r="D49" s="4">
-        <f t="shared" si="0"/>
-        <v>520503.5607086001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="7" t="s">
-        <v>1732</v>
-      </c>
-      <c r="B50" s="7">
-        <v>182263.4</v>
-      </c>
-      <c r="C50" s="5">
-        <v>182263.4</v>
-      </c>
-      <c r="D50" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="7" t="s">
-        <v>1733</v>
-      </c>
-      <c r="B51" s="7">
-        <v>247742.54452853301</v>
-      </c>
-      <c r="C51" s="4">
-        <v>251500.79999999999</v>
-      </c>
-      <c r="D51" s="4">
-        <f t="shared" si="0"/>
-        <v>-3758.2554714669823</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="7" t="s">
-        <v>1734</v>
-      </c>
-      <c r="B52" s="7">
-        <v>149387.85605758999</v>
-      </c>
-      <c r="C52" s="4">
-        <v>146602.29999999999</v>
-      </c>
-      <c r="D52" s="4">
-        <f t="shared" si="0"/>
-        <v>2785.5560575900017</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="7" t="s">
-        <v>1735</v>
-      </c>
-      <c r="B53" s="7">
-        <v>327887.29839934799</v>
-      </c>
-      <c r="C53" s="4">
-        <v>385843.3</v>
-      </c>
-      <c r="D53" s="4">
-        <f t="shared" si="0"/>
-        <v>-57956.001600652002</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="7" t="s">
-        <v>1736</v>
-      </c>
-      <c r="B54" s="7">
-        <v>325151.13489429798</v>
-      </c>
-      <c r="C54" s="4">
-        <v>379717</v>
-      </c>
-      <c r="D54" s="4">
-        <f t="shared" si="0"/>
-        <v>-54565.865105702018</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="7" t="s">
-        <v>1737</v>
-      </c>
-      <c r="B55" s="7">
-        <v>304162.99278675101</v>
-      </c>
-      <c r="C55" s="4">
-        <v>327397.8</v>
-      </c>
-      <c r="D55" s="4">
-        <f t="shared" si="0"/>
-        <v>-23234.807213248976</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="7" t="s">
-        <v>1738</v>
-      </c>
-      <c r="B56" s="7">
-        <v>187722.29999999699</v>
-      </c>
-      <c r="C56" s="4">
-        <v>187722.3</v>
-      </c>
-      <c r="D56" s="4">
-        <f t="shared" si="0"/>
-        <v>-2.9976945370435715E-9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="7" t="s">
-        <v>1739</v>
-      </c>
-      <c r="B57" s="7">
-        <v>370033.77948718</v>
-      </c>
-      <c r="C57" s="4">
-        <v>377061.7</v>
-      </c>
-      <c r="D57" s="4">
-        <f t="shared" si="0"/>
-        <v>-7027.9205128200119</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="7" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B58" s="7">
-        <v>169646.061350148</v>
-      </c>
-      <c r="C58" s="4">
-        <v>177873.5</v>
-      </c>
-      <c r="D58" s="4">
-        <f t="shared" si="0"/>
-        <v>-8227.4386498520034</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="7" t="s">
-        <v>1741</v>
-      </c>
-      <c r="B59" s="7">
-        <v>327565.22512257198</v>
-      </c>
-      <c r="C59" s="4">
-        <v>379168.7</v>
-      </c>
-      <c r="D59" s="4">
-        <f t="shared" si="0"/>
-        <v>-51603.474877428031</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="7" t="s">
-        <v>1742</v>
-      </c>
-      <c r="B60" s="7">
-        <v>231412.59129228999</v>
-      </c>
-      <c r="C60" s="4">
-        <v>202365.1</v>
-      </c>
-      <c r="D60" s="4">
-        <f t="shared" si="0"/>
-        <v>29047.491292289982</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="7" t="s">
-        <v>1743</v>
-      </c>
-      <c r="B61" s="7">
-        <v>330041.53155761398</v>
-      </c>
-      <c r="C61" s="4">
-        <v>251888.9</v>
-      </c>
-      <c r="D61" s="4">
-        <f t="shared" si="0"/>
-        <v>78152.63155761399</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="7" t="s">
-        <v>1744</v>
-      </c>
-      <c r="B62" s="7">
-        <v>187914.124263039</v>
-      </c>
-      <c r="C62" s="4">
-        <v>219906.8</v>
-      </c>
-      <c r="D62" s="4">
-        <f t="shared" si="0"/>
-        <v>-31992.675736960984</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="7" t="s">
-        <v>1745</v>
-      </c>
-      <c r="B63" s="7">
-        <v>63239.45</v>
-      </c>
-      <c r="C63" s="4">
-        <v>63239.45</v>
-      </c>
-      <c r="D63" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="7" t="s">
-        <v>1746</v>
-      </c>
-      <c r="B64" s="7">
-        <v>207404.68200887501</v>
-      </c>
-      <c r="C64" s="4">
-        <v>268204.2</v>
-      </c>
-      <c r="D64" s="4">
-        <f t="shared" si="0"/>
-        <v>-60799.517991125002</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="7" t="s">
-        <v>1747</v>
-      </c>
-      <c r="B65" s="7">
-        <v>248116.36358876101</v>
-      </c>
-      <c r="C65" s="4">
-        <v>254156.7</v>
-      </c>
-      <c r="D65" s="4">
-        <f t="shared" si="0"/>
-        <v>-6040.3364112389972</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="7" t="s">
-        <v>1748</v>
-      </c>
-      <c r="B66" s="7">
-        <v>223151.29775079599</v>
-      </c>
-      <c r="C66" s="4">
-        <v>182567.5</v>
-      </c>
-      <c r="D66" s="4">
-        <f t="shared" si="0"/>
-        <v>40583.797750795988</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="7" t="s">
-        <v>1749</v>
-      </c>
-      <c r="B67" s="7">
-        <v>256357.55055047799</v>
-      </c>
-      <c r="C67" s="4">
-        <v>262122.4</v>
-      </c>
-      <c r="D67" s="4">
-        <f t="shared" ref="D67:D73" si="3">B67-C67</f>
-        <v>-5764.8494495220075</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="7" t="s">
-        <v>1750</v>
-      </c>
-      <c r="B68" s="7">
-        <v>188034.822675737</v>
-      </c>
-      <c r="C68" s="4">
-        <v>271807.09999999998</v>
-      </c>
-      <c r="D68" s="4">
-        <f t="shared" si="3"/>
-        <v>-83772.277324262977</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="7" t="s">
-        <v>1751</v>
-      </c>
-      <c r="B69" s="7">
-        <v>134966.79999999999</v>
-      </c>
-      <c r="C69" s="4">
-        <v>134966.79999999999</v>
-      </c>
-      <c r="D69" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="7" t="s">
-        <v>1752</v>
-      </c>
-      <c r="B70" s="7">
-        <v>323187.666426257</v>
-      </c>
-      <c r="C70" s="4">
-        <v>216178.4</v>
-      </c>
-      <c r="D70" s="4">
-        <f t="shared" si="3"/>
-        <v>107009.266426257</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="7" t="s">
-        <v>1753</v>
-      </c>
-      <c r="B71" s="7">
-        <v>372762.24272085499</v>
-      </c>
-      <c r="C71" s="4">
-        <v>356538</v>
-      </c>
-      <c r="D71" s="4">
-        <f t="shared" si="3"/>
-        <v>16224.242720854993</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="7" t="s">
-        <v>1754</v>
-      </c>
-      <c r="B72" s="7">
-        <v>247742.54452853301</v>
-      </c>
-      <c r="C72" s="4">
-        <v>251192.7</v>
-      </c>
-      <c r="D72" s="4">
-        <f t="shared" si="3"/>
-        <v>-3450.1554714670056</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="7" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B73" s="7">
-        <v>230368.63951035001</v>
-      </c>
-      <c r="C73" s="4">
-        <v>164930.20000000001</v>
-      </c>
-      <c r="D73" s="4">
-        <f t="shared" si="3"/>
-        <v>65438.439510349999</v>
-      </c>
+    <row r="30" spans="1:33">
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" spans="1:33">
+      <c r="P31" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A1:XFD1048576">
+  <conditionalFormatting sqref="A1:D25 A74:XFD1048576 E49:XFD73 I26:XFD48 F2:XFD25 G1:XFD1">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>